<commit_message>
Paginas verificadas y alerta incluida
</commit_message>
<xml_diff>
--- a/Resources/datapool/DatosBookAFlight.xlsx
+++ b/Resources/datapool/DatosBookAFlight.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>Nombre del elemento</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>UNITED STATES</t>
+  </si>
+  <si>
+    <t>UKRAINE</t>
+  </si>
+  <si>
+    <t>Con este valor no se abre ninguna alerta</t>
   </si>
 </sst>
 </file>
@@ -172,7 +178,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -204,6 +210,14 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Ubuntu"/>
@@ -253,7 +267,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -275,6 +289,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -295,10 +313,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.15"/>
@@ -316,6 +334,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -324,6 +343,7 @@
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -332,6 +352,7 @@
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -340,6 +361,7 @@
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="C4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -348,6 +370,7 @@
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="C5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -356,6 +379,7 @@
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="C6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -364,6 +388,7 @@
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="C7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -372,6 +397,7 @@
       <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="C8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -380,6 +406,7 @@
       <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="C9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -388,6 +415,7 @@
       <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="C10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -396,6 +424,7 @@
       <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="C11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -404,6 +433,7 @@
       <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="C12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -412,6 +442,7 @@
       <c r="B13" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="C13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
@@ -420,6 +451,7 @@
       <c r="B14" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="C14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -428,6 +460,7 @@
       <c r="B15" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="C15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -436,6 +469,7 @@
       <c r="B16" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="C16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
@@ -444,6 +478,7 @@
       <c r="B17" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="C17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -452,6 +487,7 @@
       <c r="B18" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="C18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -460,6 +496,7 @@
       <c r="B19" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="C19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
@@ -468,6 +505,7 @@
       <c r="B20" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="C20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
@@ -476,6 +514,7 @@
       <c r="B21" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="C21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
@@ -484,6 +523,7 @@
       <c r="B22" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="C22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
@@ -492,6 +532,7 @@
       <c r="B23" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="C23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
@@ -500,6 +541,7 @@
       <c r="B24" s="4" t="s">
         <v>46</v>
       </c>
+      <c r="C24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
@@ -507,6 +549,14 @@
       </c>
       <c r="B25" s="5" t="s">
         <v>48</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reserva para multiples pasajeros
</commit_message>
<xml_diff>
--- a/Resources/datapool/DatosBookAFlight.xlsx
+++ b/Resources/datapool/DatosBookAFlight.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>Nombre del elemento</t>
   </si>
@@ -29,16 +29,43 @@
     <t>MiNombre</t>
   </si>
   <si>
+    <t>Nombre p2</t>
+  </si>
+  <si>
+    <t>Nombre p3</t>
+  </si>
+  <si>
+    <t>Nombre p4</t>
+  </si>
+  <si>
     <t>Input Last name</t>
   </si>
   <si>
     <t>MiApellido</t>
   </si>
   <si>
+    <t>Apellido p2</t>
+  </si>
+  <si>
+    <t>Apellido p3</t>
+  </si>
+  <si>
+    <t>Apellido p4</t>
+  </si>
+  <si>
     <t>Combo box Meal</t>
   </si>
   <si>
     <t>Vegetarian</t>
+  </si>
+  <si>
+    <t>Bland</t>
+  </si>
+  <si>
+    <t>Low Calorie</t>
+  </si>
+  <si>
+    <t>Diabetic</t>
   </si>
   <si>
     <t>Combo box Credit card</t>
@@ -178,7 +205,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -215,6 +242,12 @@
       <name val="Ubuntu"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
     </font>
     <font>
       <u val="single"/>
@@ -267,7 +300,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -288,11 +321,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -313,17 +350,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.762962962963"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.5851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.062962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.5962962962963"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="10.5296296296296"/>
   </cols>
   <sheetData>
@@ -343,220 +380,244 @@
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="0"/>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="0"/>
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="0"/>
+        <v>12</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="C6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="C8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>48</v>
+        <v>56</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="6" t="s">
-        <v>50</v>
+      <c r="B26" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>